<commit_message>
Standardized measurement values in the planet info spreadsheet
</commit_message>
<xml_diff>
--- a/planets_info.xlsx
+++ b/planets_info.xlsx
@@ -61,7 +61,7 @@
     <t xml:space="preserve">1,516 mi</t>
   </si>
   <si>
-    <t xml:space="preserve">3.285 × 10^23 kg</t>
+    <t xml:space="preserve">.033 × 10^25 kg</t>
   </si>
   <si>
     <t xml:space="preserve">58d 15h 30m</t>
@@ -79,13 +79,13 @@
     <t xml:space="preserve">Venus is the second planet from the Sun. It is named after the Roman goddess of love and beauty. As the second-brightest natural object in Earth's night sky after the Moon, Venus can cast shadows and can be, on rare occasion, visible to the naked eye in broad daylight.</t>
   </si>
   <si>
-    <t xml:space="preserve">67.028 million mi</t>
+    <t xml:space="preserve">67.03 million mi</t>
   </si>
   <si>
     <t xml:space="preserve">3,760.4 mi</t>
   </si>
   <si>
-    <t xml:space="preserve">4.867 × 10^24 kg</t>
+    <t xml:space="preserve">.487 × 10^25 kg</t>
   </si>
   <si>
     <t xml:space="preserve">116d 18h 0m</t>
@@ -109,7 +109,7 @@
     <t xml:space="preserve">3,958.8 mi</t>
   </si>
   <si>
-    <t xml:space="preserve">5.972 × 10^24 kg</t>
+    <t xml:space="preserve">.597 × 10^25 kg</t>
   </si>
   <si>
     <t xml:space="preserve">1d</t>
@@ -133,7 +133,7 @@
     <t xml:space="preserve">2,106.1 mi</t>
   </si>
   <si>
-    <t xml:space="preserve">6.39 × 10^23 kg</t>
+    <t xml:space="preserve">.064 × 10^25 kg</t>
   </si>
   <si>
     <t xml:space="preserve">1d 0h 37m</t>
@@ -157,7 +157,7 @@
     <t xml:space="preserve">43,441 mi</t>
   </si>
   <si>
-    <t xml:space="preserve">1.898 × 10^27 kg</t>
+    <t xml:space="preserve">189.8 × 10^25 kg</t>
   </si>
   <si>
     <t xml:space="preserve">0d 9h 56m</t>
@@ -181,7 +181,7 @@
     <t xml:space="preserve">36,184 mi</t>
   </si>
   <si>
-    <t xml:space="preserve">5.683 × 10^26 kg</t>
+    <t xml:space="preserve">56.83 × 10^25 kg</t>
   </si>
   <si>
     <t xml:space="preserve">0d 10h 42m</t>
@@ -199,7 +199,7 @@
     <t xml:space="preserve">Uranus is the seventh planet from the Sun. Its name is a reference to the Greek god of the sky, Uranus, who, according to Greek mythology, was the grandfather of Zeus and father of Cronus. It has the third-largest planetary radius and fourth-largest planetary mass in the Solar System.</t>
   </si>
   <si>
-    <t xml:space="preserve">1.784 billion mi</t>
+    <t xml:space="preserve">1,784 million mi</t>
   </si>
   <si>
     <t xml:space="preserve">15,759 mi</t>
@@ -223,13 +223,13 @@
     <t xml:space="preserve">Neptune is the eighth and farthest-known Solar planet from the Sun. In the Solar System, it is the fourth-largest planet by diameter, the third-most-massive planet, and the densest giant planet. It is 17 times the mass of Earth, slightly more massive than its near-twin Uranus.</t>
   </si>
   <si>
-    <t xml:space="preserve">2.793 billion mi</t>
+    <t xml:space="preserve">2,793 million mi</t>
   </si>
   <si>
     <t xml:space="preserve">15,299 mi</t>
   </si>
   <si>
-    <t xml:space="preserve">1.024 × 10^26 kg</t>
+    <t xml:space="preserve">10.24 × 10^25 kg</t>
   </si>
   <si>
     <t xml:space="preserve">0d 16h 6m</t>
@@ -248,11 +248,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -274,11 +275,6 @@
       <name val="Tahoma"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -323,16 +319,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -356,16 +348,18 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.36"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.06"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.19"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="14.03"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -610,7 +604,7 @@
       <c r="C9" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="1" t="s">
         <v>67</v>
       </c>
       <c r="E9" s="1" t="s">

</xml_diff>